<commit_message>
Added Photos & More sections
</commit_message>
<xml_diff>
--- a/src/local/Barhop-data.xlsx
+++ b/src/local/Barhop-data.xlsx
@@ -5,22 +5,24 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrusri/Development/code/kyrusri/winston/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrusri/Development/code/kyrusri/winston/src/local/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28720" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$M$28</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -203,12 +205,27 @@
   <si>
     <t>29-Sep</t>
   </si>
+  <si>
+    <t>Smoker Contact</t>
+  </si>
+  <si>
+    <t>Unique Trialist</t>
+  </si>
+  <si>
+    <t>Packs Sold per Sale</t>
+  </si>
+  <si>
+    <t>Unique Trialist per Smoker Contact</t>
+  </si>
+  <si>
+    <t>Smoker per Non-smoker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,8 +265,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +292,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor theme="9" tint="-0.249977111117893"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -362,11 +392,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -410,6 +469,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1484,7 +1551,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:L30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField axis="axisRow" showAll="0">
@@ -2495,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4829,4 +4896,1934 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P29" sqref="M1:P29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="21">
+        <v>132</v>
+      </c>
+      <c r="C3" s="21">
+        <v>90</v>
+      </c>
+      <c r="D3" s="21">
+        <v>683</v>
+      </c>
+      <c r="E3" s="21">
+        <v>117</v>
+      </c>
+      <c r="F3" s="21">
+        <v>60</v>
+      </c>
+      <c r="G3" s="21">
+        <v>1</v>
+      </c>
+      <c r="H3" s="21">
+        <v>0</v>
+      </c>
+      <c r="I3" s="21">
+        <v>12</v>
+      </c>
+      <c r="J3" s="21">
+        <v>147</v>
+      </c>
+      <c r="K3" s="21">
+        <v>14</v>
+      </c>
+      <c r="L3" s="21">
+        <v>234</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="24">
+        <f>L3/E3</f>
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <f>C3/B3</f>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="P3">
+        <f>B3/(D3-B3)</f>
+        <v>0.23956442831215971</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="21">
+        <v>188</v>
+      </c>
+      <c r="C4" s="21">
+        <v>107</v>
+      </c>
+      <c r="D4" s="21">
+        <v>524</v>
+      </c>
+      <c r="E4" s="21">
+        <v>60</v>
+      </c>
+      <c r="F4" s="21">
+        <v>51</v>
+      </c>
+      <c r="G4" s="21">
+        <v>17</v>
+      </c>
+      <c r="H4" s="21">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21">
+        <v>8</v>
+      </c>
+      <c r="J4" s="21">
+        <v>38</v>
+      </c>
+      <c r="K4" s="21">
+        <v>6</v>
+      </c>
+      <c r="L4" s="21">
+        <v>120</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="24">
+        <f t="shared" ref="N4:N29" si="0">L4/E4</f>
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O29" si="1">C4/B4</f>
+        <v>0.56914893617021278</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P29" si="2">B4/(D4-B4)</f>
+        <v>0.55952380952380953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="21">
+        <v>161</v>
+      </c>
+      <c r="C5" s="21">
+        <v>134</v>
+      </c>
+      <c r="D5" s="21">
+        <v>445</v>
+      </c>
+      <c r="E5" s="21">
+        <v>60</v>
+      </c>
+      <c r="F5" s="21">
+        <v>2</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>3</v>
+      </c>
+      <c r="J5" s="21">
+        <v>115</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21">
+        <v>120</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>0.83229813664596275</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>0.56690140845070425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="21">
+        <v>231</v>
+      </c>
+      <c r="C6" s="21">
+        <v>198</v>
+      </c>
+      <c r="D6" s="21">
+        <v>450</v>
+      </c>
+      <c r="E6" s="21">
+        <v>66</v>
+      </c>
+      <c r="F6" s="21">
+        <v>11</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>10</v>
+      </c>
+      <c r="I6" s="21">
+        <v>1</v>
+      </c>
+      <c r="J6" s="21">
+        <v>103</v>
+      </c>
+      <c r="K6" s="21">
+        <v>5</v>
+      </c>
+      <c r="L6" s="21">
+        <v>130</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9696969696969697</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>1.0547945205479452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="21">
+        <v>337</v>
+      </c>
+      <c r="C7" s="21">
+        <v>213</v>
+      </c>
+      <c r="D7" s="21">
+        <v>782</v>
+      </c>
+      <c r="E7" s="21">
+        <v>70</v>
+      </c>
+      <c r="F7" s="21">
+        <v>6</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
+      <c r="I7" s="21">
+        <v>2</v>
+      </c>
+      <c r="J7" s="21">
+        <v>121</v>
+      </c>
+      <c r="K7" s="21">
+        <v>10</v>
+      </c>
+      <c r="L7" s="21">
+        <v>139</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9857142857142858</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>0.63204747774480707</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>0.75730337078651688</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="21">
+        <v>181</v>
+      </c>
+      <c r="C8" s="21">
+        <v>142</v>
+      </c>
+      <c r="D8" s="21">
+        <v>542</v>
+      </c>
+      <c r="E8" s="21">
+        <v>58</v>
+      </c>
+      <c r="F8" s="21">
+        <v>6</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2</v>
+      </c>
+      <c r="H8" s="21">
+        <v>16</v>
+      </c>
+      <c r="I8" s="21">
+        <v>2</v>
+      </c>
+      <c r="J8" s="21">
+        <v>81</v>
+      </c>
+      <c r="K8" s="21">
+        <v>5</v>
+      </c>
+      <c r="L8" s="21">
+        <v>112</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9310344827586208</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>0.78453038674033149</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>0.50138504155124652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="21">
+        <v>274</v>
+      </c>
+      <c r="C9" s="21">
+        <v>235</v>
+      </c>
+      <c r="D9" s="21">
+        <v>571</v>
+      </c>
+      <c r="E9" s="21">
+        <v>82</v>
+      </c>
+      <c r="F9" s="21">
+        <v>3</v>
+      </c>
+      <c r="G9" s="21">
+        <v>1</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <v>6</v>
+      </c>
+      <c r="J9" s="21">
+        <v>131</v>
+      </c>
+      <c r="K9" s="21">
+        <v>8</v>
+      </c>
+      <c r="L9" s="21">
+        <v>149</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="24">
+        <f t="shared" si="0"/>
+        <v>1.8170731707317074</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>0.85766423357664234</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>0.92255892255892258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="21">
+        <v>276</v>
+      </c>
+      <c r="C10" s="21">
+        <v>233</v>
+      </c>
+      <c r="D10" s="21">
+        <v>548</v>
+      </c>
+      <c r="E10" s="21">
+        <v>41</v>
+      </c>
+      <c r="F10" s="21">
+        <v>6</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <v>10</v>
+      </c>
+      <c r="I10" s="21">
+        <v>11</v>
+      </c>
+      <c r="J10" s="21">
+        <v>41</v>
+      </c>
+      <c r="K10" s="21">
+        <v>12</v>
+      </c>
+      <c r="L10" s="21">
+        <v>80</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9512195121951219</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>0.84420289855072461</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>1.0147058823529411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="21">
+        <v>243</v>
+      </c>
+      <c r="C11" s="21">
+        <v>197</v>
+      </c>
+      <c r="D11" s="21">
+        <v>608</v>
+      </c>
+      <c r="E11" s="21">
+        <v>58</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0</v>
+      </c>
+      <c r="J11" s="21">
+        <v>100</v>
+      </c>
+      <c r="K11" s="21">
+        <v>12</v>
+      </c>
+      <c r="L11" s="21">
+        <v>112</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9310344827586208</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>0.81069958847736623</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>0.66575342465753429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="21">
+        <v>278</v>
+      </c>
+      <c r="C12" s="21">
+        <v>209</v>
+      </c>
+      <c r="D12" s="21">
+        <v>675</v>
+      </c>
+      <c r="E12" s="21">
+        <v>74</v>
+      </c>
+      <c r="F12" s="21">
+        <v>10</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="21">
+        <v>10</v>
+      </c>
+      <c r="I12" s="21">
+        <v>25</v>
+      </c>
+      <c r="J12" s="21">
+        <v>81</v>
+      </c>
+      <c r="K12" s="21">
+        <v>3</v>
+      </c>
+      <c r="L12" s="21">
+        <v>129</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="24">
+        <f t="shared" si="0"/>
+        <v>1.7432432432432432</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>0.75179856115107913</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>0.7002518891687658</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="21">
+        <v>282</v>
+      </c>
+      <c r="C13" s="21">
+        <v>228</v>
+      </c>
+      <c r="D13" s="21">
+        <v>512</v>
+      </c>
+      <c r="E13" s="21">
+        <v>55</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
+      <c r="G13" s="21">
+        <v>1</v>
+      </c>
+      <c r="H13" s="21">
+        <v>3</v>
+      </c>
+      <c r="I13" s="21">
+        <v>6</v>
+      </c>
+      <c r="J13" s="21">
+        <v>90</v>
+      </c>
+      <c r="K13" s="21">
+        <v>7</v>
+      </c>
+      <c r="L13" s="21">
+        <v>107</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9454545454545455</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>0.80851063829787229</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>1.2260869565217392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="21">
+        <v>313</v>
+      </c>
+      <c r="C14" s="21">
+        <v>251</v>
+      </c>
+      <c r="D14" s="21">
+        <v>523</v>
+      </c>
+      <c r="E14" s="21">
+        <v>51</v>
+      </c>
+      <c r="F14" s="21">
+        <v>20</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>12</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="21">
+        <v>69</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0</v>
+      </c>
+      <c r="L14" s="21">
+        <v>101</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9803921568627452</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>0.80191693290734822</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>1.4904761904761905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="21">
+        <v>299</v>
+      </c>
+      <c r="C15" s="21">
+        <v>244</v>
+      </c>
+      <c r="D15" s="21">
+        <v>498</v>
+      </c>
+      <c r="E15" s="21">
+        <v>62</v>
+      </c>
+      <c r="F15" s="21">
+        <v>4</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0</v>
+      </c>
+      <c r="H15" s="21">
+        <v>8</v>
+      </c>
+      <c r="I15" s="21">
+        <v>0</v>
+      </c>
+      <c r="J15" s="21">
+        <v>104</v>
+      </c>
+      <c r="K15" s="21">
+        <v>8</v>
+      </c>
+      <c r="L15" s="21">
+        <v>124</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>0.81605351170568563</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="2"/>
+        <v>1.5025125628140703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="21">
+        <v>419</v>
+      </c>
+      <c r="C16" s="21">
+        <v>355</v>
+      </c>
+      <c r="D16" s="21">
+        <v>659</v>
+      </c>
+      <c r="E16" s="21">
+        <v>41</v>
+      </c>
+      <c r="F16" s="21">
+        <v>3</v>
+      </c>
+      <c r="G16" s="21">
+        <v>5</v>
+      </c>
+      <c r="H16" s="21">
+        <v>1</v>
+      </c>
+      <c r="I16" s="21">
+        <v>1</v>
+      </c>
+      <c r="J16" s="21">
+        <v>68</v>
+      </c>
+      <c r="K16" s="21">
+        <v>3</v>
+      </c>
+      <c r="L16" s="21">
+        <v>81</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" si="0"/>
+        <v>1.975609756097561</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="1"/>
+        <v>0.847255369928401</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="2"/>
+        <v>1.7458333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="21">
+        <v>339</v>
+      </c>
+      <c r="C17" s="21">
+        <v>264</v>
+      </c>
+      <c r="D17" s="21">
+        <v>598</v>
+      </c>
+      <c r="E17" s="21">
+        <v>53</v>
+      </c>
+      <c r="F17" s="21">
+        <v>11</v>
+      </c>
+      <c r="G17" s="21">
+        <v>0</v>
+      </c>
+      <c r="H17" s="21">
+        <v>11</v>
+      </c>
+      <c r="I17" s="21">
+        <v>10</v>
+      </c>
+      <c r="J17" s="21">
+        <v>72</v>
+      </c>
+      <c r="K17" s="21">
+        <v>1</v>
+      </c>
+      <c r="L17" s="21">
+        <v>105</v>
+      </c>
+      <c r="M17" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>0.77876106194690264</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="2"/>
+        <v>1.3088803088803089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="21">
+        <v>313</v>
+      </c>
+      <c r="C18" s="21">
+        <v>248</v>
+      </c>
+      <c r="D18" s="21">
+        <v>516</v>
+      </c>
+      <c r="E18" s="21">
+        <v>46</v>
+      </c>
+      <c r="F18" s="21">
+        <v>7</v>
+      </c>
+      <c r="G18" s="21">
+        <v>0</v>
+      </c>
+      <c r="H18" s="21">
+        <v>10</v>
+      </c>
+      <c r="I18" s="21">
+        <v>4</v>
+      </c>
+      <c r="J18" s="21">
+        <v>66</v>
+      </c>
+      <c r="K18" s="21">
+        <v>5</v>
+      </c>
+      <c r="L18" s="21">
+        <v>92</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>0.792332268370607</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="2"/>
+        <v>1.541871921182266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="21">
+        <v>343</v>
+      </c>
+      <c r="C19" s="21">
+        <v>229</v>
+      </c>
+      <c r="D19" s="21">
+        <v>542</v>
+      </c>
+      <c r="E19" s="21">
+        <v>91</v>
+      </c>
+      <c r="F19" s="21">
+        <v>30</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0</v>
+      </c>
+      <c r="H19" s="21">
+        <v>30</v>
+      </c>
+      <c r="I19" s="21">
+        <v>3</v>
+      </c>
+      <c r="J19" s="21">
+        <v>104</v>
+      </c>
+      <c r="K19" s="21">
+        <v>5</v>
+      </c>
+      <c r="L19" s="21">
+        <v>172</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="0"/>
+        <v>1.8901098901098901</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="1"/>
+        <v>0.66763848396501457</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="2"/>
+        <v>1.7236180904522613</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="21">
+        <v>367</v>
+      </c>
+      <c r="C20" s="21">
+        <v>261</v>
+      </c>
+      <c r="D20" s="21">
+        <v>516</v>
+      </c>
+      <c r="E20" s="21">
+        <v>39</v>
+      </c>
+      <c r="F20" s="21">
+        <v>2</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0</v>
+      </c>
+      <c r="H20" s="21">
+        <v>0</v>
+      </c>
+      <c r="I20" s="21">
+        <v>3</v>
+      </c>
+      <c r="J20" s="21">
+        <v>67</v>
+      </c>
+      <c r="K20" s="21">
+        <v>6</v>
+      </c>
+      <c r="L20" s="21">
+        <v>78</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>0.71117166212534055</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>2.4630872483221475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="21">
+        <v>424</v>
+      </c>
+      <c r="C21" s="21">
+        <v>270</v>
+      </c>
+      <c r="D21" s="21">
+        <v>720</v>
+      </c>
+      <c r="E21" s="21">
+        <v>53</v>
+      </c>
+      <c r="F21" s="21">
+        <v>10</v>
+      </c>
+      <c r="G21" s="21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="21">
+        <v>1</v>
+      </c>
+      <c r="I21" s="21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="21">
+        <v>86</v>
+      </c>
+      <c r="K21" s="21">
+        <v>8</v>
+      </c>
+      <c r="L21" s="21">
+        <v>105</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" s="24">
+        <f t="shared" si="0"/>
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>0.6367924528301887</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>1.4324324324324325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="21">
+        <v>415</v>
+      </c>
+      <c r="C22" s="21">
+        <v>282</v>
+      </c>
+      <c r="D22" s="21">
+        <v>630</v>
+      </c>
+      <c r="E22" s="21">
+        <v>47</v>
+      </c>
+      <c r="F22" s="21">
+        <v>13</v>
+      </c>
+      <c r="G22" s="21">
+        <v>4</v>
+      </c>
+      <c r="H22" s="21">
+        <v>14</v>
+      </c>
+      <c r="I22" s="21">
+        <v>0</v>
+      </c>
+      <c r="J22" s="21">
+        <v>59</v>
+      </c>
+      <c r="K22" s="21">
+        <v>4</v>
+      </c>
+      <c r="L22" s="21">
+        <v>94</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>0.67951807228915662</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>1.930232558139535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="21">
+        <v>454</v>
+      </c>
+      <c r="C23" s="21">
+        <v>308</v>
+      </c>
+      <c r="D23" s="21">
+        <v>535</v>
+      </c>
+      <c r="E23" s="21">
+        <v>49</v>
+      </c>
+      <c r="F23" s="21">
+        <v>4</v>
+      </c>
+      <c r="G23" s="21">
+        <v>0</v>
+      </c>
+      <c r="H23" s="21">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21">
+        <v>2</v>
+      </c>
+      <c r="J23" s="21">
+        <v>85</v>
+      </c>
+      <c r="K23" s="21">
+        <v>7</v>
+      </c>
+      <c r="L23" s="21">
+        <v>98</v>
+      </c>
+      <c r="M23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>0.67841409691629961</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>5.6049382716049383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="21">
+        <v>359</v>
+      </c>
+      <c r="C24" s="21">
+        <v>226</v>
+      </c>
+      <c r="D24" s="21">
+        <v>597</v>
+      </c>
+      <c r="E24" s="21">
+        <v>40</v>
+      </c>
+      <c r="F24" s="21">
+        <v>10</v>
+      </c>
+      <c r="G24" s="21">
+        <v>0</v>
+      </c>
+      <c r="H24" s="21">
+        <v>12</v>
+      </c>
+      <c r="I24" s="21">
+        <v>0</v>
+      </c>
+      <c r="J24" s="21">
+        <v>39</v>
+      </c>
+      <c r="K24" s="21">
+        <v>19</v>
+      </c>
+      <c r="L24" s="21">
+        <v>80</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="N24" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>0.62952646239554322</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>1.5084033613445378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="21">
+        <v>403</v>
+      </c>
+      <c r="C25" s="21">
+        <v>356</v>
+      </c>
+      <c r="D25" s="21">
+        <v>628</v>
+      </c>
+      <c r="E25" s="21">
+        <v>115</v>
+      </c>
+      <c r="F25" s="21">
+        <v>21</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0</v>
+      </c>
+      <c r="H25" s="21">
+        <v>50</v>
+      </c>
+      <c r="I25" s="21">
+        <v>1</v>
+      </c>
+      <c r="J25" s="21">
+        <v>140</v>
+      </c>
+      <c r="K25" s="21">
+        <v>3</v>
+      </c>
+      <c r="L25" s="21">
+        <v>215</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="24">
+        <f t="shared" si="0"/>
+        <v>1.8695652173913044</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>0.88337468982630274</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>1.7911111111111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="21">
+        <v>342</v>
+      </c>
+      <c r="C26" s="21">
+        <v>324</v>
+      </c>
+      <c r="D26" s="21">
+        <v>487</v>
+      </c>
+      <c r="E26" s="21">
+        <v>46</v>
+      </c>
+      <c r="F26" s="21">
+        <v>5</v>
+      </c>
+      <c r="G26" s="21">
+        <v>0</v>
+      </c>
+      <c r="H26" s="21">
+        <v>0</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
+      <c r="J26" s="21">
+        <v>81</v>
+      </c>
+      <c r="K26" s="21">
+        <v>6</v>
+      </c>
+      <c r="L26" s="21">
+        <v>92</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="N26" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>2.3586206896551722</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="21">
+        <v>336</v>
+      </c>
+      <c r="C27" s="21">
+        <v>288</v>
+      </c>
+      <c r="D27" s="21">
+        <v>587</v>
+      </c>
+      <c r="E27" s="21">
+        <v>69</v>
+      </c>
+      <c r="F27" s="21">
+        <v>12</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0</v>
+      </c>
+      <c r="H27" s="21">
+        <v>16</v>
+      </c>
+      <c r="I27" s="21">
+        <v>0</v>
+      </c>
+      <c r="J27" s="21">
+        <v>103</v>
+      </c>
+      <c r="K27" s="21">
+        <v>7</v>
+      </c>
+      <c r="L27" s="21">
+        <v>138</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N27" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>1.3386454183266931</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="21">
+        <v>295</v>
+      </c>
+      <c r="C28" s="21">
+        <v>231</v>
+      </c>
+      <c r="D28" s="21">
+        <v>507</v>
+      </c>
+      <c r="E28" s="21">
+        <v>110</v>
+      </c>
+      <c r="F28" s="21">
+        <v>56</v>
+      </c>
+      <c r="G28" s="21">
+        <v>0</v>
+      </c>
+      <c r="H28" s="21">
+        <v>30</v>
+      </c>
+      <c r="I28" s="21">
+        <v>5</v>
+      </c>
+      <c r="J28" s="21">
+        <v>78</v>
+      </c>
+      <c r="K28" s="21">
+        <v>2</v>
+      </c>
+      <c r="L28" s="21">
+        <v>171</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N28" s="24">
+        <f t="shared" si="0"/>
+        <v>1.5545454545454545</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>0.7830508474576271</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>1.3915094339622642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="21">
+        <v>346</v>
+      </c>
+      <c r="C29" s="21">
+        <v>243</v>
+      </c>
+      <c r="D29" s="21">
+        <v>534</v>
+      </c>
+      <c r="E29" s="21">
+        <v>36</v>
+      </c>
+      <c r="F29" s="21">
+        <v>14</v>
+      </c>
+      <c r="G29" s="21">
+        <v>0</v>
+      </c>
+      <c r="H29" s="21">
+        <v>10</v>
+      </c>
+      <c r="I29" s="21">
+        <v>0</v>
+      </c>
+      <c r="J29" s="21">
+        <v>44</v>
+      </c>
+      <c r="K29" s="21">
+        <v>4</v>
+      </c>
+      <c r="L29" s="21">
+        <v>72</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0.70231213872832365</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>1.8404255319148937</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="D3">
+        <v>0.23956442831215971</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.56914893617021278</v>
+      </c>
+      <c r="D4">
+        <v>0.55952380952380953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0.83229813664596275</v>
+      </c>
+      <c r="D5">
+        <v>0.56690140845070425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>1.9696969696969697</v>
+      </c>
+      <c r="C6">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D6">
+        <v>1.0547945205479452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>1.9857142857142858</v>
+      </c>
+      <c r="C7">
+        <v>0.63204747774480707</v>
+      </c>
+      <c r="D7">
+        <v>0.75730337078651688</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>1.9310344827586208</v>
+      </c>
+      <c r="C8">
+        <v>0.78453038674033149</v>
+      </c>
+      <c r="D8">
+        <v>0.50138504155124652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>1.8170731707317074</v>
+      </c>
+      <c r="C9">
+        <v>0.85766423357664234</v>
+      </c>
+      <c r="D9">
+        <v>0.92255892255892258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>1.9512195121951219</v>
+      </c>
+      <c r="C10">
+        <v>0.84420289855072461</v>
+      </c>
+      <c r="D10">
+        <v>1.0147058823529411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>1.9310344827586208</v>
+      </c>
+      <c r="C11">
+        <v>0.81069958847736623</v>
+      </c>
+      <c r="D11">
+        <v>0.66575342465753429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>1.7432432432432432</v>
+      </c>
+      <c r="C12">
+        <v>0.75179856115107913</v>
+      </c>
+      <c r="D12">
+        <v>0.7002518891687658</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>1.9454545454545455</v>
+      </c>
+      <c r="C13">
+        <v>0.80851063829787229</v>
+      </c>
+      <c r="D13">
+        <v>1.2260869565217392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>1.9803921568627452</v>
+      </c>
+      <c r="C14">
+        <v>0.80191693290734822</v>
+      </c>
+      <c r="D14">
+        <v>1.4904761904761905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0.81605351170568563</v>
+      </c>
+      <c r="D15">
+        <v>1.5025125628140703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>1.975609756097561</v>
+      </c>
+      <c r="C16">
+        <v>0.847255369928401</v>
+      </c>
+      <c r="D16">
+        <v>1.7458333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="C17">
+        <v>0.77876106194690264</v>
+      </c>
+      <c r="D17">
+        <v>1.3088803088803089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>0.792332268370607</v>
+      </c>
+      <c r="D18">
+        <v>1.541871921182266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19">
+        <v>1.8901098901098901</v>
+      </c>
+      <c r="C19">
+        <v>0.66763848396501457</v>
+      </c>
+      <c r="D19">
+        <v>1.7236180904522613</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>0.71117166212534055</v>
+      </c>
+      <c r="D20">
+        <v>2.4630872483221475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21">
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="C21">
+        <v>0.6367924528301887</v>
+      </c>
+      <c r="D21">
+        <v>1.4324324324324325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0.67951807228915662</v>
+      </c>
+      <c r="D22">
+        <v>1.930232558139535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>0.67841409691629961</v>
+      </c>
+      <c r="D23">
+        <v>5.6049382716049383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>0.62952646239554322</v>
+      </c>
+      <c r="D24">
+        <v>1.5084033613445378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25">
+        <v>1.8695652173913044</v>
+      </c>
+      <c r="C25">
+        <v>0.88337468982630274</v>
+      </c>
+      <c r="D25">
+        <v>1.7911111111111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="D26">
+        <v>2.3586206896551722</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D27">
+        <v>1.3386454183266931</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28">
+        <v>1.5545454545454545</v>
+      </c>
+      <c r="C28">
+        <v>0.7830508474576271</v>
+      </c>
+      <c r="D28">
+        <v>1.3915094339622642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>0.70231213872832365</v>
+      </c>
+      <c r="D29">
+        <v>1.8404255319148937</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>